<commit_message>
Moved commintment spreadsheet from Documents to Budget
</commit_message>
<xml_diff>
--- a/docs/budget/effort_committment.xlsx
+++ b/docs/budget/effort_committment.xlsx
@@ -1112,7 +1112,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="9">
         <f>SUM(E35:L37)</f>
-        <v>367.8</v>
+        <v>292.275</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1148,7 +1148,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="11">
         <f>SUM(E35:H37)</f>
-        <v>176.4</v>
+        <v>136.05</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>19</v>
@@ -1157,7 +1157,7 @@
       <c r="K18" s="10"/>
       <c r="L18" s="11">
         <f>SUM(I35:L37)</f>
-        <v>191.4</v>
+        <v>156.225</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>29</v>
@@ -1172,7 +1172,7 @@
       <c r="U18" s="12"/>
       <c r="V18" s="13">
         <f>SUM(M35:V37)</f>
-        <v>387.7125</v>
+        <v>372.7125</v>
       </c>
       <c r="W18" s="14" t="s">
         <v>30</v>
@@ -1598,16 +1598,16 @@
         <v>20</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L24" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M24" s="19" t="s">
         <v>23</v>
@@ -1622,10 +1622,10 @@
         <v>20</v>
       </c>
       <c r="Q24" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="S24" s="20" t="s">
         <v>20</v>
@@ -1659,15 +1659,15 @@
       </c>
       <c r="AD24" s="3">
         <f t="shared" ref="AD24:AD33" si="4">COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
-        <v>0</v>
+        <v>50.4375</v>
       </c>
       <c r="AE24" s="3">
         <f t="shared" ref="AE24:AE33" si="5">COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
-        <v>286.6625</v>
+        <v>211.225</v>
       </c>
       <c r="AF24" s="3">
         <f t="shared" ref="AF24:AF33" si="6">SUM(AC24:AE24)</f>
-        <v>286.6625</v>
+        <v>261.6625</v>
       </c>
       <c r="AG24" s="1"/>
     </row>
@@ -1679,10 +1679,10 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="21" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>16</v>
@@ -1702,10 +1702,10 @@
       <c r="L25" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M25" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="N25" s="22" t="s">
         <v>23</v>
       </c>
       <c r="O25" s="1" t="s">
@@ -1715,22 +1715,22 @@
         <v>16</v>
       </c>
       <c r="Q25" s="22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="R25" s="22" t="s">
         <v>16</v>
       </c>
       <c r="S25" s="22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T25" s="22" t="s">
         <v>16</v>
       </c>
       <c r="U25" s="22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="V25" s="22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="W25" s="22" t="s">
         <v>16</v>
@@ -1748,19 +1748,19 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="3">
         <f t="shared" si="3"/>
-        <v>5.0875</v>
+        <v>15.2625</v>
       </c>
       <c r="AD25" s="3">
         <f t="shared" si="4"/>
-        <v>171.4875</v>
+        <v>121.05</v>
       </c>
       <c r="AE25" s="3">
         <f t="shared" si="5"/>
-        <v>15.0875</v>
+        <v>30.175</v>
       </c>
       <c r="AF25" s="3">
         <f t="shared" si="6"/>
-        <v>191.6625</v>
+        <v>166.4875</v>
       </c>
       <c r="AG25" s="1"/>
     </row>
@@ -1781,10 +1781,10 @@
         <v>16</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J26" s="21" t="s">
         <v>16</v>
@@ -1793,10 +1793,10 @@
         <v>16</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N26" s="23" t="s">
         <v>16</v>
@@ -1865,22 +1865,22 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>16</v>
@@ -1901,13 +1901,13 @@
         <v>16</v>
       </c>
       <c r="Q27" s="22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R27" s="22" t="s">
         <v>16</v>
       </c>
       <c r="S27" s="22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="T27" s="22" t="s">
         <v>16</v>
@@ -1934,19 +1934,19 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10.175</v>
       </c>
       <c r="AD27" s="3">
         <f t="shared" si="4"/>
-        <v>191.6625</v>
+        <v>110.9625</v>
       </c>
       <c r="AE27" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>30.175</v>
       </c>
       <c r="AF27" s="3">
         <f t="shared" si="6"/>
-        <v>191.6625</v>
+        <v>151.3125</v>
       </c>
       <c r="AG27" s="1"/>
     </row>
@@ -2555,15 +2555,15 @@
       </c>
       <c r="E35" s="3">
         <f t="shared" ref="E35:Z35" si="7">COUNTIFS(E$24:E$34,$I9) * $F$9</f>
-        <v>5.0875</v>
+        <v>0</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0875</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0875</v>
       </c>
       <c r="H35" s="3">
         <f t="shared" si="7"/>
@@ -2603,7 +2603,7 @@
       </c>
       <c r="Q35" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0875</v>
       </c>
       <c r="R35" s="3">
         <f t="shared" si="7"/>
@@ -2619,11 +2619,11 @@
       </c>
       <c r="U35" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0875</v>
       </c>
       <c r="V35" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>5.0875</v>
       </c>
       <c r="W35" s="3">
         <f t="shared" si="7"/>
@@ -2659,39 +2659,39 @@
       </c>
       <c r="E36" s="3">
         <f t="shared" ref="E36:Z36" si="9">COUNTIFS(E$24:E$34,$I10) * $F$10</f>
-        <v>20.175</v>
+        <v>10.0875</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="9"/>
-        <v>30.2625</v>
+        <v>10.0875</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="9"/>
-        <v>30.2625</v>
+        <v>20.175</v>
       </c>
       <c r="H36" s="3">
         <f t="shared" si="9"/>
-        <v>30.2625</v>
+        <v>10.0875</v>
       </c>
       <c r="I36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>10.0875</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="9"/>
-        <v>30.2625</v>
+        <v>20.175</v>
       </c>
       <c r="K36" s="3">
         <f t="shared" si="9"/>
-        <v>30.2625</v>
+        <v>40.35</v>
       </c>
       <c r="L36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>40.35</v>
       </c>
       <c r="M36" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10.0875</v>
       </c>
       <c r="N36" s="3">
         <f t="shared" si="9"/>
@@ -2707,15 +2707,15 @@
       </c>
       <c r="Q36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>10.0875</v>
       </c>
       <c r="R36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>30.2625</v>
       </c>
       <c r="S36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>0</v>
       </c>
       <c r="T36" s="3">
         <f t="shared" si="9"/>
@@ -2723,11 +2723,11 @@
       </c>
       <c r="U36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>10.0875</v>
       </c>
       <c r="V36" s="3">
         <f t="shared" si="9"/>
-        <v>20.175</v>
+        <v>10.0875</v>
       </c>
       <c r="W36" s="3">
         <f t="shared" si="9"/>
@@ -2751,19 +2751,19 @@
       </c>
       <c r="AC36" s="16">
         <f t="shared" ref="AC36:AF36" si="10">SUM(AC24:AC34)</f>
-        <v>5.0875</v>
+        <v>25.4375</v>
       </c>
       <c r="AD36" s="16">
         <f t="shared" si="10"/>
-        <v>494.2875</v>
+        <v>413.5875</v>
       </c>
       <c r="AE36" s="16">
         <f t="shared" si="10"/>
-        <v>437.5375</v>
+        <v>407.3625</v>
       </c>
       <c r="AF36" s="16">
         <f t="shared" si="10"/>
-        <v>936.9125</v>
+        <v>846.3875</v>
       </c>
       <c r="AG36" s="16" t="s">
         <v>4</v>
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H37" s="3">
         <f t="shared" si="11"/>
-        <v>15.0875</v>
+        <v>30.175</v>
       </c>
       <c r="I37" s="3">
         <f t="shared" si="11"/>
@@ -2803,15 +2803,15 @@
       </c>
       <c r="K37" s="3">
         <f t="shared" si="11"/>
-        <v>15.0875</v>
+        <v>0</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="11"/>
-        <v>30.175</v>
+        <v>0</v>
       </c>
       <c r="M37" s="3">
         <f t="shared" si="11"/>
-        <v>15.0875</v>
+        <v>0</v>
       </c>
       <c r="N37" s="3">
         <f t="shared" si="11"/>
@@ -2831,11 +2831,11 @@
       </c>
       <c r="R37" s="3">
         <f t="shared" si="11"/>
-        <v>30.175</v>
+        <v>15.0875</v>
       </c>
       <c r="S37" s="3">
         <f t="shared" si="11"/>
-        <v>30.175</v>
+        <v>60.35</v>
       </c>
       <c r="T37" s="3">
         <f t="shared" si="11"/>
@@ -3024,39 +3024,39 @@
       </c>
       <c r="E42" s="3">
         <f t="shared" ref="E42:Z42" si="12">SUM(E35:E37)</f>
-        <v>40.35</v>
+        <v>25.175</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="12"/>
-        <v>45.35</v>
+        <v>30.2625</v>
       </c>
       <c r="G42" s="3">
         <f t="shared" si="12"/>
-        <v>45.35</v>
+        <v>40.35</v>
       </c>
       <c r="H42" s="3">
         <f t="shared" si="12"/>
-        <v>45.35</v>
+        <v>40.2625</v>
       </c>
       <c r="I42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>40.2625</v>
       </c>
       <c r="J42" s="3">
         <f t="shared" si="12"/>
-        <v>45.35</v>
+        <v>35.2625</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="12"/>
-        <v>45.35</v>
+        <v>40.35</v>
       </c>
       <c r="L42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>40.35</v>
       </c>
       <c r="M42" s="3">
         <f t="shared" si="12"/>
-        <v>15.0875</v>
+        <v>10.0875</v>
       </c>
       <c r="N42" s="3">
         <f t="shared" si="12"/>
@@ -3072,15 +3072,15 @@
       </c>
       <c r="Q42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>45.35</v>
       </c>
       <c r="R42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>45.35</v>
       </c>
       <c r="S42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>60.35</v>
       </c>
       <c r="T42" s="3">
         <f t="shared" si="12"/>
@@ -3088,11 +3088,11 @@
       </c>
       <c r="U42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>45.35</v>
       </c>
       <c r="V42" s="3">
         <f t="shared" si="12"/>
-        <v>50.35</v>
+        <v>45.35</v>
       </c>
       <c r="W42" s="3">
         <f t="shared" si="12"/>
@@ -3118,7 +3118,7 @@
       <c r="AD42" s="16"/>
       <c r="AE42" s="16">
         <f>SUM(E42:Z42)</f>
-        <v>936.9125</v>
+        <v>846.3875</v>
       </c>
       <c r="AF42" s="16"/>
       <c r="AG42" s="16" t="s">
@@ -3137,27 +3137,27 @@
       <c r="E43" s="3"/>
       <c r="F43" s="3">
         <f>SUM(E42:F42)</f>
-        <v>85.7</v>
+        <v>55.4375</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3">
         <f>SUM(G42:H42)</f>
-        <v>90.7</v>
+        <v>80.6125</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3">
         <f>SUM(I42:J42)</f>
-        <v>95.7</v>
+        <v>75.525</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3">
         <f>SUM(K42:L42)</f>
-        <v>95.7</v>
+        <v>80.7</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3">
         <f>SUM(M42:N42)</f>
-        <v>25.175</v>
+        <v>20.175</v>
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3">
@@ -3167,17 +3167,17 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="3">
         <f>SUM(Q42:R42)</f>
-        <v>100.7</v>
+        <v>90.7</v>
       </c>
       <c r="S43" s="3"/>
       <c r="T43" s="3">
         <f>SUM(S42:T42)</f>
-        <v>100.7</v>
+        <v>110.7</v>
       </c>
       <c r="U43" s="3"/>
       <c r="V43" s="3">
         <f>SUM(U42:V42)</f>
-        <v>100.7</v>
+        <v>90.7</v>
       </c>
       <c r="W43" s="3"/>
       <c r="X43" s="3">
@@ -3197,7 +3197,7 @@
       <c r="AD43" s="16"/>
       <c r="AE43" s="16">
         <f>SUM(D43:Z43)</f>
-        <v>936.9125</v>
+        <v>846.3875</v>
       </c>
       <c r="AF43" s="3"/>
       <c r="AG43" s="16" t="s">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="C47" s="30">
         <f>AE43</f>
-        <v>936.9125</v>
+        <v>846.3875</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>49</v>

</xml_diff>